<commit_message>
Update Institusjonell sektorgruppering 2012.xlsx
</commit_message>
<xml_diff>
--- a/Institusjonell sektorgruppering 2012.xlsx
+++ b/Institusjonell sektorgruppering 2012.xlsx
@@ -1355,10 +1355,11 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101005BAF6522D6B39A4F809F4AA1655E5CD6" ma:contentTypeVersion="12" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="e4a524b860cf13a8c93835716f8e4da0">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="712f17e0-2077-4e3f-8ea2-c75d02de46ee" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="810e635cb89f261f8aa95246a976651c" ns1:_="" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101005BAF6522D6B39A4F809F4AA1655E5CD6" ma:contentTypeVersion="15" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="5d2df7d88173eed2472aac31f58c6f9b">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="712f17e0-2077-4e3f-8ea2-c75d02de46ee" xmlns:ns3="4c1e125b-b772-4d2d-8af8-eec310c9bc7c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="020ddd7b595e894bbf41ffe05b9a61ec" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="712f17e0-2077-4e3f-8ea2-c75d02de46ee"/>
+    <xsd:import namespace="4c1e125b-b772-4d2d-8af8-eec310c9bc7c"/>
     <xsd:element name="properties">
       <xsd:complexType>
         <xsd:sequence>
@@ -1378,6 +1379,8 @@
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1460,6 +1463,28 @@
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="22" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Bildemerkelapper" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="17f1e631-7134-4ce3-8a3d-482fd88a4c57" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="4c1e125b-b772-4d2d-8af8-eec310c9bc7c" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="23" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{cfd1b471-962e-4074-a3f5-f81efd63bd54}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="a65edee0-4267-4101-9877-75c307db3846">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -1566,6 +1591,10 @@
   <documentManagement>
     <PublishingExpirationDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <PublishingStartDate xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="4c1e125b-b772-4d2d-8af8-eec310c9bc7c" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="712f17e0-2077-4e3f-8ea2-c75d02de46ee">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
 </file>
@@ -1579,22 +1608,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A37B37-1A59-4161-8B44-BCBD3E747F56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="712f17e0-2077-4e3f-8ea2-c75d02de46ee"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0B21BE4-BB33-4812-803E-132CDF67D025}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>